<commit_message>
adding HoH gender to strata variables
</commit_message>
<xml_diff>
--- a/EduAnalysisTool/input_tool/edu_indicator_labelling.xlsx
+++ b/EduAnalysisTool/input_tool/edu_indicator_labelling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/MSNA_2024_EduAnalysis/EduAnalysisTool/input_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{4971C11D-3DCB-447F-9F3B-182DA7D1D740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{783439DF-0402-4988-987B-AB93609C8802}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:1_{4971C11D-3DCB-447F-9F3B-182DA7D1D740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6257168E-6E5E-4BD0-9241-7855866413B6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="update_survey" sheetId="6" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="200">
   <si>
     <t>theme</t>
   </si>
@@ -232,12 +232,6 @@
     <t>% d'enfants non scolarisés ou en éducation pré-primaire en 2023-2024, par raison principale</t>
   </si>
   <si>
-    <t>% d'enfants avec 2 ans de plus que l'âge prévu : primaire</t>
-  </si>
-  <si>
-    <t>% d'enfants avec 2 ans de plus que l'âge prévu : secondaire</t>
-  </si>
-  <si>
     <t>% d'enfants accédant à l'éducation en dehors des écoles formelles en 2023-2024, par type de programme</t>
   </si>
   <si>
@@ -415,9 +409,6 @@
     <t>% of school-aged children attending primary school who are at least 2 years above the intended age for their grade</t>
   </si>
   <si>
-    <t>% of school-aged children attending secondary school who are at least 2 years above the intended age for their grade</t>
-  </si>
-  <si>
     <t>% of school-aged children whose education was disrupted due to the school being occupied by displaced persons</t>
   </si>
   <si>
@@ -598,9 +589,6 @@
     <t>% of school-aged children accessing education outside of formal schools during the 2023-2024 school year</t>
   </si>
   <si>
-    <t>% of school-aged children accessing education outside of formal schools during the 2023-2024 school year, by type of program attended</t>
-  </si>
-  <si>
     <t>edu_access_only_formal</t>
   </si>
   <si>
@@ -616,19 +604,46 @@
     <t>edu_access_formal_OR_nonformal</t>
   </si>
   <si>
-    <t>% children 5 to 18 y.o. who attended either formal school or structured non-formal school</t>
-  </si>
-  <si>
-    <t>% children 5 to 18 y.o. who attended formal school only</t>
-  </si>
-  <si>
-    <t>% children 5 to 18 y.o. who attended non-formal school only</t>
-  </si>
-  <si>
-    <t>% children 5 to 18 y.o. who attended formal school AND non-formal school</t>
-  </si>
-  <si>
-    <t>% children 5 to 18 y.o. who attended either formal school or non-formal school</t>
+    <t>edu_level3_overage_learners_d</t>
+  </si>
+  <si>
+    <t>edu_attending_level12_and_level1_age_d</t>
+  </si>
+  <si>
+    <t>edu_attending_level2_and_level2_age_d</t>
+  </si>
+  <si>
+    <t>% d'enfants d'âge scolaire fréquentant le enseignement secondaire general ou technique qui ont au moins deux ans de plus que l'âge prévu pour leur classe</t>
+  </si>
+  <si>
+    <t>% d'enfants d'âge scolaire fréquentant l'enseignement fondamental 1 qui ont au moins deux ans de plus que l'âge prévu pour leur classe</t>
+  </si>
+  <si>
+    <t>% d'enfants d'âge scolaire fréquentant l'enseignement fondamental 2 qui ont au moins deux ans de plus que l'âge prévu pour leur classe</t>
+  </si>
+  <si>
+    <t>by type of program attended, % of school-aged children accessing education outside of formal schools during the 2023-2024 school year</t>
+  </si>
+  <si>
+    <t>% of school-aged children attending lower secondary school who are at least 2 years above the intended age for their grade</t>
+  </si>
+  <si>
+    <t>% of school-aged children attending  upper secondary school who are at least 2 years above the intended age for their grade</t>
+  </si>
+  <si>
+    <t>formal school only</t>
+  </si>
+  <si>
+    <t>non-formal school only</t>
+  </si>
+  <si>
+    <t>either formal school or structured non-formal school</t>
+  </si>
+  <si>
+    <t>formal school AND non-formal school</t>
+  </si>
+  <si>
+    <t>either formal school or non-formal school</t>
   </si>
 </sst>
 </file>
@@ -715,7 +730,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -734,15 +749,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1011,17 +1025,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.75" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.5" style="7" customWidth="1"/>
+    <col min="2" max="2" width="17.75" style="7" customWidth="1"/>
     <col min="3" max="3" width="41.75" style="7" customWidth="1"/>
     <col min="4" max="4" width="94.875" style="7" customWidth="1"/>
     <col min="5" max="5" width="52.25" style="7" customWidth="1"/>
@@ -1058,7 +1072,7 @@
       <c r="D2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1075,7 +1089,7 @@
       <c r="D3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1092,7 +1106,7 @@
       <c r="D4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1109,8 +1123,8 @@
       <c r="D5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>143</v>
+      <c r="E5" s="7" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1126,7 +1140,7 @@
       <c r="D6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1141,10 +1155,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>144</v>
+        <v>121</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1160,8 +1174,8 @@
       <c r="D8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>181</v>
+      <c r="E8" s="7" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1177,7 +1191,7 @@
       <c r="D9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1191,11 +1205,11 @@
       <c r="C10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1209,10 +1223,10 @@
         <v>26</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1223,12 +1237,12 @@
         <v>6</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>27</v>
+        <v>187</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1240,12 +1254,12 @@
         <v>6</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>28</v>
+        <v>188</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1257,13 +1271,13 @@
         <v>6</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>58</v>
+        <v>46</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1274,13 +1288,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>56</v>
+        <v>44</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1291,13 +1305,13 @@
         <v>6</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>59</v>
+        <v>45</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1308,13 +1322,13 @@
         <v>6</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>58</v>
+        <v>46</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1325,13 +1339,13 @@
         <v>6</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>60</v>
+        <v>44</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1339,16 +1353,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>182</v>
+        <v>6</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>61</v>
+        <v>47</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1359,13 +1373,13 @@
         <v>6</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>62</v>
+        <v>48</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1373,50 +1387,50 @@
         <v>1</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>6</v>
+        <v>179</v>
       </c>
       <c r="C21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>64</v>
+      <c r="D23" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1427,16 +1441,16 @@
         <v>6</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>34</v>
+        <v>186</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>1</v>
       </c>
@@ -1444,30 +1458,30 @@
         <v>6</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>125</v>
+        <v>36</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>164</v>
+        <v>142</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>192</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>179</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1477,14 +1491,14 @@
       <c r="B27" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>165</v>
+      <c r="C27" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>180</v>
+        <v>33</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1495,13 +1509,13 @@
         <v>6</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>171</v>
+        <v>122</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>123</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>175</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1512,10 +1526,10 @@
         <v>6</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>172</v>
+        <v>160</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>161</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>176</v>
@@ -1529,10 +1543,10 @@
         <v>6</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>173</v>
+        <v>162</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>163</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>177</v>
@@ -1546,13 +1560,13 @@
         <v>6</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>174</v>
+        <v>164</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>168</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1563,66 +1577,117 @@
         <v>6</v>
       </c>
       <c r="C32" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>194</v>
+      <c r="D39" s="7" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -1683,245 +1748,245 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>22</v>
@@ -1935,139 +2000,139 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>24</v>
@@ -2075,30 +2140,30 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>